<commit_message>
Update validation scenario, inverter and year default
</commit_message>
<xml_diff>
--- a/tests/validation_scenario_0/Outputs/ProForma.xlsx
+++ b/tests/validation_scenario_0/Outputs/ProForma.xlsx
@@ -495,14 +495,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="26.7109375" customWidth="1"/>
-    <col min="2" max="27" width="10.7109375" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="22" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -710,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>14.5278</v>
+        <v>29.6131</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.41932</v>
+        <v>1.69242</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -726,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.335456</v>
+        <v>1.35394</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>2160</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -766,10 +766,10 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -777,7 +777,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -785,36 +785,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1882</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+        <v>2818</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -881,23 +881,8 @@
       <c r="V24">
         <v>20</v>
       </c>
-      <c r="W24">
-        <v>21</v>
-      </c>
-      <c r="X24">
-        <v>22</v>
-      </c>
-      <c r="Y24">
-        <v>23</v>
-      </c>
-      <c r="Z24">
-        <v>24</v>
-      </c>
-      <c r="AA24">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -906,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -990,28 +975,8 @@
         <f>-$B$16*$B$9*(1+$B$7)^V24</f>
         <v>0</v>
       </c>
-      <c r="W26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^W24</f>
-        <v>0</v>
-      </c>
-      <c r="X26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^X24</f>
-        <v>0</v>
-      </c>
-      <c r="Y26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^Y24</f>
-        <v>0</v>
-      </c>
-      <c r="Z26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^Z24</f>
-        <v>0</v>
-      </c>
-      <c r="AA26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^AA24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1020,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1104,28 +1069,8 @@
         <f>$B$19*(1+$B$6)^V24</f>
         <v>0</v>
       </c>
-      <c r="W28" s="2">
-        <f>$B$19*(1+$B$6)^W24</f>
-        <v>0</v>
-      </c>
-      <c r="X28" s="2">
-        <f>$B$19*(1+$B$6)^X24</f>
-        <v>0</v>
-      </c>
-      <c r="Y28" s="2">
-        <f>$B$19*(1+$B$6)^Y24</f>
-        <v>0</v>
-      </c>
-      <c r="Z28" s="2">
-        <f>$B$19*(1+$B$6)^Z24</f>
-        <v>0</v>
-      </c>
-      <c r="AA28" s="2">
-        <f>$B$19*(1+$B$6)^AA24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1209,28 +1154,8 @@
         <f>$B$20*(1+$B$6)^V24</f>
         <v>0</v>
       </c>
-      <c r="W29" s="2">
-        <f>$B$20*(1+$B$6)^W24</f>
-        <v>0</v>
-      </c>
-      <c r="X29" s="2">
-        <f>$B$20*(1+$B$6)^X24</f>
-        <v>0</v>
-      </c>
-      <c r="Y29" s="2">
-        <f>$B$20*(1+$B$6)^Y24</f>
-        <v>0</v>
-      </c>
-      <c r="Z29" s="2">
-        <f>$B$20*(1+$B$6)^Z24</f>
-        <v>0</v>
-      </c>
-      <c r="AA29" s="2">
-        <f>$B$20*(1+$B$6)^AA24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1259,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1277,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1361,28 +1286,8 @@
         <f>(1-$B$3)*(V28+V29)</f>
         <v>0</v>
       </c>
-      <c r="W33" s="2">
-        <f>(1-$B$3)*(W28+W29)</f>
-        <v>0</v>
-      </c>
-      <c r="X33" s="2">
-        <f>(1-$B$3)*(X28+X29)</f>
-        <v>0</v>
-      </c>
-      <c r="Y33" s="2">
-        <f>(1-$B$3)*(Y28+Y29)</f>
-        <v>0</v>
-      </c>
-      <c r="Z33" s="2">
-        <f>(1-$B$3)*(Z28+Z29)</f>
-        <v>0</v>
-      </c>
-      <c r="AA33" s="2">
-        <f>(1-$B$3)*(AA28+AA29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1466,28 +1371,8 @@
         <f>(1-$B$3)*V26</f>
         <v>0</v>
       </c>
-      <c r="W34" s="2">
-        <f>(1-$B$3)*W26</f>
-        <v>0</v>
-      </c>
-      <c r="X34" s="2">
-        <f>(1-$B$3)*X26</f>
-        <v>0</v>
-      </c>
-      <c r="Y34" s="2">
-        <f>(1-$B$3)*Y26</f>
-        <v>0</v>
-      </c>
-      <c r="Z34" s="2">
-        <f>(1-$B$3)*Z26</f>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="2">
-        <f>(1-$B$3)*AA26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1575,28 +1460,8 @@
         <f>V25+V27+SUM(V30:V34)</f>
         <v>0</v>
       </c>
-      <c r="W35" s="2">
-        <f>W25+W27+SUM(W30:W34)</f>
-        <v>0</v>
-      </c>
-      <c r="X35" s="2">
-        <f>X25+X27+SUM(X30:X34)</f>
-        <v>0</v>
-      </c>
-      <c r="Y35" s="2">
-        <f>Y25+Y27+SUM(Y30:Y34)</f>
-        <v>0</v>
-      </c>
-      <c r="Z35" s="2">
-        <f>Z25+Z27+SUM(Z30:Z34)</f>
-        <v>0</v>
-      </c>
-      <c r="AA35" s="2">
-        <f>AA25+AA27+SUM(AA30:AA34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1684,33 +1549,13 @@
         <f>V35/(1+$B$2)^V24</f>
         <v>0</v>
       </c>
-      <c r="W36" s="2">
-        <f>W35/(1+$B$2)^W24</f>
-        <v>0</v>
-      </c>
-      <c r="X36" s="2">
-        <f>X35/(1+$B$2)^X24</f>
-        <v>0</v>
-      </c>
-      <c r="Y36" s="2">
-        <f>Y35/(1+$B$2)^Y24</f>
-        <v>0</v>
-      </c>
-      <c r="Z36" s="2">
-        <f>Z35/(1+$B$2)^Z24</f>
-        <v>0</v>
-      </c>
-      <c r="AA36" s="2">
-        <f>AA35/(1+$B$2)^AA24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1719,13 +1564,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="3">
         <f>IRR(B35:AA35)</f>
-        <v>0.148853699701</v>
+        <v>0.148125190255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pv max size constraint, validation
</commit_message>
<xml_diff>
--- a/tests/validation_scenario_0/Outputs/ProForma.xlsx
+++ b/tests/validation_scenario_0/Outputs/ProForma.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>Inputs can be changed here</t>
   </si>
@@ -67,7 +67,10 @@
     <t>PV 0&amp;M ($/kW/yr)</t>
   </si>
   <si>
-    <t>Battery replacement cost</t>
+    <t>Battery replacement cost ($/kWh)</t>
+  </si>
+  <si>
+    <t>Inverter replacement cost ($/kW)</t>
   </si>
   <si>
     <t>Year 1 energy savings</t>
@@ -76,6 +79,12 @@
     <t>Year 1 demand savings</t>
   </si>
   <si>
+    <t>Year 1 export benefit</t>
+  </si>
+  <si>
+    <t>PV degradation (%/year)</t>
+  </si>
+  <si>
     <t>analysis_period</t>
   </si>
   <si>
@@ -88,13 +97,16 @@
     <t>O&amp;M (PV)</t>
   </si>
   <si>
-    <t>Battery Replacement</t>
-  </si>
-  <si>
-    <t>Energy Cost Savings</t>
-  </si>
-  <si>
-    <t>Demand Cost Savings</t>
+    <t>Battery Replacement Cost</t>
+  </si>
+  <si>
+    <t>Energy Bill Savings</t>
+  </si>
+  <si>
+    <t>Demand Bill Savings</t>
+  </si>
+  <si>
+    <t>Energy Export Benefit</t>
   </si>
   <si>
     <t>Depreciation Tax Shield</t>
@@ -106,7 +118,7 @@
     <t>Bonus Tax Shield</t>
   </si>
   <si>
-    <t>After Tax Electricity Savings</t>
+    <t>After Tax Bill Savings</t>
   </si>
   <si>
     <t>After Tax O&amp;M</t>
@@ -125,6 +137,12 @@
   </si>
   <si>
     <t>IRR</t>
+  </si>
+  <si>
+    <t>LCC (with system)</t>
+  </si>
+  <si>
+    <t>LCC (without system)</t>
   </si>
   <si>
     <t>MACRS schedule</t>
@@ -495,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -521,14 +539,14 @@
         <v>0.1295500000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2">
-        <f>-B25-0.5*C31</f>
+        <f>-B28-0.5*C35</f>
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -539,7 +557,7 @@
         <v>0.35</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -568,7 +586,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>0.2</v>
@@ -597,7 +615,7 @@
         <v>0.3</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -608,7 +626,7 @@
         <v>0.02899750000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2">
         <f>E2-B4*E2</f>
@@ -643,7 +661,7 @@
         <v>0.025</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F7" s="2">
         <f>$F$6*F4</f>
@@ -678,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F8" s="2">
         <f>F6-F7</f>
@@ -710,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>22.9427</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -718,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.15</v>
+        <v>0.790461</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -726,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.12</v>
+        <v>0.632369</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -779,18 +797,18 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -798,7 +816,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>27</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -806,267 +824,112 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="1" t="s">
-        <v>2</v>
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0.005</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <v>4</v>
-      </c>
-      <c r="G24">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>6</v>
-      </c>
-      <c r="I24">
-        <v>7</v>
-      </c>
-      <c r="J24">
-        <v>8</v>
-      </c>
-      <c r="K24">
-        <v>9</v>
-      </c>
-      <c r="L24">
-        <v>10</v>
-      </c>
-      <c r="M24">
-        <v>11</v>
-      </c>
-      <c r="N24">
-        <v>12</v>
-      </c>
-      <c r="O24">
-        <v>13</v>
-      </c>
-      <c r="P24">
-        <v>14</v>
-      </c>
-      <c r="Q24">
-        <v>15</v>
-      </c>
-      <c r="R24">
-        <v>16</v>
-      </c>
-      <c r="S24">
-        <v>17</v>
-      </c>
-      <c r="T24">
-        <v>18</v>
-      </c>
-      <c r="U24">
-        <v>19</v>
-      </c>
-      <c r="V24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2">
-        <f>-(B9*B13+B10*B14+B11*B15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^C24</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^D24</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^E24</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^F24</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^G24</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^H24</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^I24</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^J24</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^K24</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^L24</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^M24</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^N24</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^O24</f>
-        <v>0</v>
-      </c>
-      <c r="P26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^P24</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^Q24</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^R24</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^S24</f>
-        <v>0</v>
-      </c>
-      <c r="T26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^T24</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^U24</f>
-        <v>0</v>
-      </c>
-      <c r="V26" s="2">
-        <f>-$B$16*$B$9*(1+$B$7)^V24</f>
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="2">
-        <f>-B17*(B10+B11)</f>
-        <v>0</v>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <v>10</v>
+      </c>
+      <c r="M27">
+        <v>11</v>
+      </c>
+      <c r="N27">
+        <v>12</v>
+      </c>
+      <c r="O27">
+        <v>13</v>
+      </c>
+      <c r="P27">
+        <v>14</v>
+      </c>
+      <c r="Q27">
+        <v>15</v>
+      </c>
+      <c r="R27">
+        <v>16</v>
+      </c>
+      <c r="S27">
+        <v>17</v>
+      </c>
+      <c r="T27">
+        <v>18</v>
+      </c>
+      <c r="U27">
+        <v>19</v>
+      </c>
+      <c r="V27">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <f>$B$19*(1+$B$6)^C24</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
-        <f>$B$19*(1+$B$6)^D24</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <f>$B$19*(1+$B$6)^E24</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <f>$B$19*(1+$B$6)^F24</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
-        <f>$B$19*(1+$B$6)^G24</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <f>$B$19*(1+$B$6)^H24</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <f>$B$19*(1+$B$6)^I24</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="2">
-        <f>$B$19*(1+$B$6)^J24</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="2">
-        <f>$B$19*(1+$B$6)^K24</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="2">
-        <f>$B$19*(1+$B$6)^L24</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="2">
-        <f>$B$19*(1+$B$6)^M24</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="2">
-        <f>$B$19*(1+$B$6)^N24</f>
-        <v>0</v>
-      </c>
-      <c r="O28" s="2">
-        <f>$B$19*(1+$B$6)^O24</f>
-        <v>0</v>
-      </c>
-      <c r="P28" s="2">
-        <f>$B$19*(1+$B$6)^P24</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="2">
-        <f>$B$19*(1+$B$6)^Q24</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="2">
-        <f>$B$19*(1+$B$6)^R24</f>
-        <v>0</v>
-      </c>
-      <c r="S28" s="2">
-        <f>$B$19*(1+$B$6)^S24</f>
-        <v>0</v>
-      </c>
-      <c r="T28" s="2">
-        <f>$B$19*(1+$B$6)^T24</f>
-        <v>0</v>
-      </c>
-      <c r="U28" s="2">
-        <f>$B$19*(1+$B$6)^U24</f>
-        <v>0</v>
-      </c>
-      <c r="V28" s="2">
-        <f>$B$19*(1+$B$6)^V24</f>
+      <c r="B28" s="2">
+        <f>-(B9*B13+B10*B14+B11*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -1075,83 +938,83 @@
         <v>26</v>
       </c>
       <c r="C29" s="2">
-        <f>$B$20*(1+$B$6)^C24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^C27</f>
         <v>0</v>
       </c>
       <c r="D29" s="2">
-        <f>$B$20*(1+$B$6)^D24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^D27</f>
         <v>0</v>
       </c>
       <c r="E29" s="2">
-        <f>$B$20*(1+$B$6)^E24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^E27</f>
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <f>$B$20*(1+$B$6)^F24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^F27</f>
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <f>$B$20*(1+$B$6)^G24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^G27</f>
         <v>0</v>
       </c>
       <c r="H29" s="2">
-        <f>$B$20*(1+$B$6)^H24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^H27</f>
         <v>0</v>
       </c>
       <c r="I29" s="2">
-        <f>$B$20*(1+$B$6)^I24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^I27</f>
         <v>0</v>
       </c>
       <c r="J29" s="2">
-        <f>$B$20*(1+$B$6)^J24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^J27</f>
         <v>0</v>
       </c>
       <c r="K29" s="2">
-        <f>$B$20*(1+$B$6)^K24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^K27</f>
         <v>0</v>
       </c>
       <c r="L29" s="2">
-        <f>$B$20*(1+$B$6)^L24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^L27</f>
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <f>$B$20*(1+$B$6)^M24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^M27</f>
         <v>0</v>
       </c>
       <c r="N29" s="2">
-        <f>$B$20*(1+$B$6)^N24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^N27</f>
         <v>0</v>
       </c>
       <c r="O29" s="2">
-        <f>$B$20*(1+$B$6)^O24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^O27</f>
         <v>0</v>
       </c>
       <c r="P29" s="2">
-        <f>$B$20*(1+$B$6)^P24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^P27</f>
         <v>0</v>
       </c>
       <c r="Q29" s="2">
-        <f>$B$20*(1+$B$6)^Q24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^Q27</f>
         <v>0</v>
       </c>
       <c r="R29" s="2">
-        <f>$B$20*(1+$B$6)^R24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^R27</f>
         <v>0</v>
       </c>
       <c r="S29" s="2">
-        <f>$B$20*(1+$B$6)^S24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^S27</f>
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <f>$B$20*(1+$B$6)^T24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^T27</f>
         <v>0</v>
       </c>
       <c r="U29" s="2">
-        <f>$B$20*(1+$B$6)^U24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^U27</f>
         <v>0</v>
       </c>
       <c r="V29" s="2">
-        <f>$B$20*(1+$B$6)^V24</f>
+        <f>-$B$16*$B$9*(1+$B$7)^V27</f>
         <v>0</v>
       </c>
     </row>
@@ -1159,28 +1022,8 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
-        <f>$B$3*F7</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <f>$B$3*G7</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <f>$B$3*H7</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <f>$B$3*I7</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <f>$B$3*J7</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <f>$B$3*K7</f>
+      <c r="L30" s="2">
+        <f>-(B10*B17+B11*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -1189,7 +1032,83 @@
         <v>28</v>
       </c>
       <c r="C31" s="2">
-        <f>-B5*B25</f>
+        <f>$B$20*(1+$B$6)^C27</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f>$B$20*(1+$B$6)^D27</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f>$B$20*(1+$B$6)^E27</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <f>$B$20*(1+$B$6)^F27</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <f>$B$20*(1+$B$6)^G27</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <f>$B$20*(1+$B$6)^H27</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <f>$B$20*(1+$B$6)^I27</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <f>$B$20*(1+$B$6)^J27</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <f>$B$20*(1+$B$6)^K27</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <f>$B$20*(1+$B$6)^L27</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <f>$B$20*(1+$B$6)^M27</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="2">
+        <f>$B$20*(1+$B$6)^N27</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="2">
+        <f>$B$20*(1+$B$6)^O27</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="2">
+        <f>$B$20*(1+$B$6)^P27</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>$B$20*(1+$B$6)^Q27</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="2">
+        <f>$B$20*(1+$B$6)^R27</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="2">
+        <f>$B$20*(1+$B$6)^S27</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="2">
+        <f>$B$20*(1+$B$6)^T27</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="2">
+        <f>$B$20*(1+$B$6)^U27</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="2">
+        <f>$B$20*(1+$B$6)^V27</f>
         <v>0</v>
       </c>
     </row>
@@ -1198,7 +1117,83 @@
         <v>29</v>
       </c>
       <c r="C32" s="2">
-        <f>E2*B4*B3</f>
+        <f>$B$21*(1+$B$6)^C27</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f>$B$21*(1+$B$6)^D27</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <f>$B$21*(1+$B$6)^E27</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <f>$B$21*(1+$B$6)^F27</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <f>$B$21*(1+$B$6)^G27</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <f>$B$21*(1+$B$6)^H27</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <f>$B$21*(1+$B$6)^I27</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <f>$B$21*(1+$B$6)^J27</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <f>$B$21*(1+$B$6)^K27</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <f>$B$21*(1+$B$6)^L27</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <f>$B$21*(1+$B$6)^M27</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="2">
+        <f>$B$21*(1+$B$6)^N27</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="2">
+        <f>$B$21*(1+$B$6)^O27</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="2">
+        <f>$B$21*(1+$B$6)^P27</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="2">
+        <f>$B$21*(1+$B$6)^Q27</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="2">
+        <f>$B$21*(1+$B$6)^R27</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="2">
+        <f>$B$21*(1+$B$6)^S27</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="2">
+        <f>$B$21*(1+$B$6)^T27</f>
+        <v>0</v>
+      </c>
+      <c r="U32" s="2">
+        <f>$B$21*(1+$B$6)^U27</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="2">
+        <f>$B$21*(1+$B$6)^V27</f>
         <v>0</v>
       </c>
     </row>
@@ -1207,83 +1202,83 @@
         <v>30</v>
       </c>
       <c r="C33" s="2">
-        <f>(1-$B$3)*(C28+C29)</f>
+        <f>$B$22*(1+$B$6)^C27*(1-$B$23)^B27</f>
         <v>0</v>
       </c>
       <c r="D33" s="2">
-        <f>(1-$B$3)*(D28+D29)</f>
+        <f>$B$22*(1+$B$6)^D27*(1-$B$23)^C27</f>
         <v>0</v>
       </c>
       <c r="E33" s="2">
-        <f>(1-$B$3)*(E28+E29)</f>
+        <f>$B$22*(1+$B$6)^E27*(1-$B$23)^D27</f>
         <v>0</v>
       </c>
       <c r="F33" s="2">
-        <f>(1-$B$3)*(F28+F29)</f>
+        <f>$B$22*(1+$B$6)^F27*(1-$B$23)^E27</f>
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f>(1-$B$3)*(G28+G29)</f>
+        <f>$B$22*(1+$B$6)^G27*(1-$B$23)^F27</f>
         <v>0</v>
       </c>
       <c r="H33" s="2">
-        <f>(1-$B$3)*(H28+H29)</f>
+        <f>$B$22*(1+$B$6)^H27*(1-$B$23)^G27</f>
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <f>(1-$B$3)*(I28+I29)</f>
+        <f>$B$22*(1+$B$6)^I27*(1-$B$23)^H27</f>
         <v>0</v>
       </c>
       <c r="J33" s="2">
-        <f>(1-$B$3)*(J28+J29)</f>
+        <f>$B$22*(1+$B$6)^J27*(1-$B$23)^I27</f>
         <v>0</v>
       </c>
       <c r="K33" s="2">
-        <f>(1-$B$3)*(K28+K29)</f>
+        <f>$B$22*(1+$B$6)^K27*(1-$B$23)^J27</f>
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <f>(1-$B$3)*(L28+L29)</f>
+        <f>$B$22*(1+$B$6)^L27*(1-$B$23)^K27</f>
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <f>(1-$B$3)*(M28+M29)</f>
+        <f>$B$22*(1+$B$6)^M27*(1-$B$23)^L27</f>
         <v>0</v>
       </c>
       <c r="N33" s="2">
-        <f>(1-$B$3)*(N28+N29)</f>
+        <f>$B$22*(1+$B$6)^N27*(1-$B$23)^M27</f>
         <v>0</v>
       </c>
       <c r="O33" s="2">
-        <f>(1-$B$3)*(O28+O29)</f>
+        <f>$B$22*(1+$B$6)^O27*(1-$B$23)^N27</f>
         <v>0</v>
       </c>
       <c r="P33" s="2">
-        <f>(1-$B$3)*(P28+P29)</f>
+        <f>$B$22*(1+$B$6)^P27*(1-$B$23)^O27</f>
         <v>0</v>
       </c>
       <c r="Q33" s="2">
-        <f>(1-$B$3)*(Q28+Q29)</f>
+        <f>$B$22*(1+$B$6)^Q27*(1-$B$23)^P27</f>
         <v>0</v>
       </c>
       <c r="R33" s="2">
-        <f>(1-$B$3)*(R28+R29)</f>
+        <f>$B$22*(1+$B$6)^R27*(1-$B$23)^Q27</f>
         <v>0</v>
       </c>
       <c r="S33" s="2">
-        <f>(1-$B$3)*(S28+S29)</f>
+        <f>$B$22*(1+$B$6)^S27*(1-$B$23)^R27</f>
         <v>0</v>
       </c>
       <c r="T33" s="2">
-        <f>(1-$B$3)*(T28+T29)</f>
+        <f>$B$22*(1+$B$6)^T27*(1-$B$23)^S27</f>
         <v>0</v>
       </c>
       <c r="U33" s="2">
-        <f>(1-$B$3)*(U28+U29)</f>
+        <f>$B$22*(1+$B$6)^U27*(1-$B$23)^T27</f>
         <v>0</v>
       </c>
       <c r="V33" s="2">
-        <f>(1-$B$3)*(V28+V29)</f>
+        <f>$B$22*(1+$B$6)^V27*(1-$B$23)^U27</f>
         <v>0</v>
       </c>
     </row>
@@ -1292,83 +1287,27 @@
         <v>31</v>
       </c>
       <c r="C34" s="2">
-        <f>(1-$B$3)*C26</f>
+        <f>$B$3*F7</f>
         <v>0</v>
       </c>
       <c r="D34" s="2">
-        <f>(1-$B$3)*D26</f>
+        <f>$B$3*G7</f>
         <v>0</v>
       </c>
       <c r="E34" s="2">
-        <f>(1-$B$3)*E26</f>
+        <f>$B$3*H7</f>
         <v>0</v>
       </c>
       <c r="F34" s="2">
-        <f>(1-$B$3)*F26</f>
+        <f>$B$3*I7</f>
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f>(1-$B$3)*G26</f>
+        <f>$B$3*J7</f>
         <v>0</v>
       </c>
       <c r="H34" s="2">
-        <f>(1-$B$3)*H26</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="2">
-        <f>(1-$B$3)*I26</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="2">
-        <f>(1-$B$3)*J26</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="2">
-        <f>(1-$B$3)*K26</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="2">
-        <f>(1-$B$3)*L26</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="2">
-        <f>(1-$B$3)*M26</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="2">
-        <f>(1-$B$3)*N26</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="2">
-        <f>(1-$B$3)*O26</f>
-        <v>0</v>
-      </c>
-      <c r="P34" s="2">
-        <f>(1-$B$3)*P26</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="2">
-        <f>(1-$B$3)*Q26</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="2">
-        <f>(1-$B$3)*R26</f>
-        <v>0</v>
-      </c>
-      <c r="S34" s="2">
-        <f>(1-$B$3)*S26</f>
-        <v>0</v>
-      </c>
-      <c r="T34" s="2">
-        <f>(1-$B$3)*T26</f>
-        <v>0</v>
-      </c>
-      <c r="U34" s="2">
-        <f>(1-$B$3)*U26</f>
-        <v>0</v>
-      </c>
-      <c r="V34" s="2">
-        <f>(1-$B$3)*V26</f>
+        <f>$B$3*K7</f>
         <v>0</v>
       </c>
     </row>
@@ -1376,88 +1315,8 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="2">
-        <f>B25+B27+SUM(B30:B34)</f>
-        <v>0</v>
-      </c>
       <c r="C35" s="2">
-        <f>C25+C27+SUM(C30:C34)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2">
-        <f>D25+D27+SUM(D30:D34)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <f>E25+E27+SUM(E30:E34)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <f>F25+F27+SUM(F30:F34)</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="2">
-        <f>G25+G27+SUM(G30:G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="2">
-        <f>H25+H27+SUM(H30:H34)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="2">
-        <f>I25+I27+SUM(I30:I34)</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="2">
-        <f>J25+J27+SUM(J30:J34)</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="2">
-        <f>K25+K27+SUM(K30:K34)</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="2">
-        <f>L25+L27+SUM(L30:L34)</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="2">
-        <f>M25+M27+SUM(M30:M34)</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="2">
-        <f>N25+N27+SUM(N30:N34)</f>
-        <v>0</v>
-      </c>
-      <c r="O35" s="2">
-        <f>O25+O27+SUM(O30:O34)</f>
-        <v>0</v>
-      </c>
-      <c r="P35" s="2">
-        <f>P25+P27+SUM(P30:P34)</f>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="2">
-        <f>Q25+Q27+SUM(Q30:Q34)</f>
-        <v>0</v>
-      </c>
-      <c r="R35" s="2">
-        <f>R25+R27+SUM(R30:R34)</f>
-        <v>0</v>
-      </c>
-      <c r="S35" s="2">
-        <f>S25+S27+SUM(S30:S34)</f>
-        <v>0</v>
-      </c>
-      <c r="T35" s="2">
-        <f>T25+T27+SUM(T30:T34)</f>
-        <v>0</v>
-      </c>
-      <c r="U35" s="2">
-        <f>U25+U27+SUM(U30:U34)</f>
-        <v>0</v>
-      </c>
-      <c r="V35" s="2">
-        <f>V25+V27+SUM(V30:V34)</f>
+        <f>-B5*B28</f>
         <v>0</v>
       </c>
     </row>
@@ -1465,88 +1324,8 @@
       <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="2">
-        <f>B35</f>
-        <v>0</v>
-      </c>
       <c r="C36" s="2">
-        <f>C35/(1+$B$2)^C24</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <f>D35/(1+$B$2)^D24</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="2">
-        <f>E35/(1+$B$2)^E24</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <f>F35/(1+$B$2)^F24</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="2">
-        <f>G35/(1+$B$2)^G24</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="2">
-        <f>H35/(1+$B$2)^H24</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="2">
-        <f>I35/(1+$B$2)^I24</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="2">
-        <f>J35/(1+$B$2)^J24</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="2">
-        <f>K35/(1+$B$2)^K24</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="2">
-        <f>L35/(1+$B$2)^L24</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="2">
-        <f>M35/(1+$B$2)^M24</f>
-        <v>0</v>
-      </c>
-      <c r="N36" s="2">
-        <f>N35/(1+$B$2)^N24</f>
-        <v>0</v>
-      </c>
-      <c r="O36" s="2">
-        <f>O35/(1+$B$2)^O24</f>
-        <v>0</v>
-      </c>
-      <c r="P36" s="2">
-        <f>P35/(1+$B$2)^P24</f>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="2">
-        <f>Q35/(1+$B$2)^Q24</f>
-        <v>0</v>
-      </c>
-      <c r="R36" s="2">
-        <f>R35/(1+$B$2)^R24</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="2">
-        <f>S35/(1+$B$2)^S24</f>
-        <v>0</v>
-      </c>
-      <c r="T36" s="2">
-        <f>T35/(1+$B$2)^T24</f>
-        <v>0</v>
-      </c>
-      <c r="U36" s="2">
-        <f>U35/(1+$B$2)^U24</f>
-        <v>0</v>
-      </c>
-      <c r="V36" s="2">
-        <f>V35/(1+$B$2)^V24</f>
+        <f>E2*B4*B3</f>
         <v>0</v>
       </c>
     </row>
@@ -1554,13 +1333,169 @@
       <c r="A37" t="s">
         <v>34</v>
       </c>
+      <c r="C37" s="2">
+        <f>(1-$B$3)*(C31+C32+C33)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f>(1-$B$3)*(D31+D32+D33)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <f>(1-$B$3)*(E31+E32+E33)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <f>(1-$B$3)*(F31+F32+F33)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <f>(1-$B$3)*(G31+G32+G33)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <f>(1-$B$3)*(H31+H32+H33)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <f>(1-$B$3)*(I31+I32+I33)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <f>(1-$B$3)*(J31+J32+J33)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <f>(1-$B$3)*(K31+K32+K33)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <f>(1-$B$3)*(L31+L32+L33)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <f>(1-$B$3)*(M31+M32+M33)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <f>(1-$B$3)*(N31+N32+N33)</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="2">
+        <f>(1-$B$3)*(O31+O32+O33)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <f>(1-$B$3)*(P31+P32+P33)</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
+        <f>(1-$B$3)*(Q31+Q32+Q33)</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="2">
+        <f>(1-$B$3)*(R31+R32+R33)</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="2">
+        <f>(1-$B$3)*(S31+S32+S33)</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="2">
+        <f>(1-$B$3)*(T31+T32+T33)</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="2">
+        <f>(1-$B$3)*(U31+U32+U33)</f>
+        <v>0</v>
+      </c>
+      <c r="V37" s="2">
+        <f>(1-$B$3)*(V31+V32+V33)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="2">
-        <f>SUM(B36:AA36)</f>
+      <c r="C38" s="2">
+        <f>(1-$B$3)*C29</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <f>(1-$B$3)*D29</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <f>(1-$B$3)*E29</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <f>(1-$B$3)*F29</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <f>(1-$B$3)*G29</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <f>(1-$B$3)*H29</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <f>(1-$B$3)*I29</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <f>(1-$B$3)*J29</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <f>(1-$B$3)*K29</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="2">
+        <f>(1-$B$3)*L29</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
+        <f>(1-$B$3)*M29</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="2">
+        <f>(1-$B$3)*N29</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="2">
+        <f>(1-$B$3)*O29</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="2">
+        <f>(1-$B$3)*P29</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="2">
+        <f>(1-$B$3)*Q29</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="2">
+        <f>(1-$B$3)*R29</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="2">
+        <f>(1-$B$3)*S29</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="2">
+        <f>(1-$B$3)*T29</f>
+        <v>0</v>
+      </c>
+      <c r="U38" s="2">
+        <f>(1-$B$3)*U29</f>
+        <v>0</v>
+      </c>
+      <c r="V38" s="2">
+        <f>(1-$B$3)*V29</f>
         <v>0</v>
       </c>
     </row>
@@ -1568,9 +1503,217 @@
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="3">
-        <f>IRR(B35:AA35)</f>
-        <v>0.138491903368</v>
+      <c r="B39" s="2">
+        <f>B28+B30+SUM(B34:B38)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C28+C30+SUM(C34:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <f>D28+D30+SUM(D34:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <f>E28+E30+SUM(E34:E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <f>F28+F30+SUM(F34:F38)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <f>G28+G30+SUM(G34:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <f>H28+H30+SUM(H34:H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <f>I28+I30+SUM(I34:I38)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <f>J28+J30+SUM(J34:J38)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <f>K28+K30+SUM(K34:K38)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <f>L28+L30+SUM(L34:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <f>M28+M30+SUM(M34:M38)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <f>N28+N30+SUM(N34:N38)</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <f>O28+O30+SUM(O34:O38)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="2">
+        <f>P28+P30+SUM(P34:P38)</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2">
+        <f>Q28+Q30+SUM(Q34:Q38)</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="2">
+        <f>R28+R30+SUM(R34:R38)</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <f>S28+S30+SUM(S34:S38)</f>
+        <v>0</v>
+      </c>
+      <c r="T39" s="2">
+        <f>T28+T30+SUM(T34:T38)</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="2">
+        <f>U28+U30+SUM(U34:U38)</f>
+        <v>0</v>
+      </c>
+      <c r="V39" s="2">
+        <f>V28+V30+SUM(V34:V38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="2">
+        <f>B39</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C39/(1+$B$2)^C27</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <f>D39/(1+$B$2)^D27</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <f>E39/(1+$B$2)^E27</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <f>F39/(1+$B$2)^F27</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <f>G39/(1+$B$2)^G27</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <f>H39/(1+$B$2)^H27</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <f>I39/(1+$B$2)^I27</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <f>J39/(1+$B$2)^J27</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <f>K39/(1+$B$2)^K27</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <f>L39/(1+$B$2)^L27</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <f>M39/(1+$B$2)^M27</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="2">
+        <f>N39/(1+$B$2)^N27</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="2">
+        <f>O39/(1+$B$2)^O27</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="2">
+        <f>P39/(1+$B$2)^P27</f>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2">
+        <f>Q39/(1+$B$2)^Q27</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="2">
+        <f>R39/(1+$B$2)^R27</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="2">
+        <f>S39/(1+$B$2)^S27</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="2">
+        <f>T39/(1+$B$2)^T27</f>
+        <v>0</v>
+      </c>
+      <c r="U40" s="2">
+        <f>U39/(1+$B$2)^U27</f>
+        <v>0</v>
+      </c>
+      <c r="V40" s="2">
+        <f>V39/(1+$B$2)^V27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="2">
+        <f>SUM(B40:V40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="3">
+        <f>IRR(B39:V39)</f>
+        <v>0.149144626775</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="2">
+        <v>414311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="2">
+        <v>418155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>